<commit_message>
Fixed issue #21 Generada medida municipio en 05-0709-070902 (en vez de refArea)
</commit_message>
<xml_diff>
--- a/data/metadata/Informe-05-0709-070902-A-TM-TC-TP.xlsx
+++ b/data/metadata/Informe-05-0709-070902-A-TM-TC-TP.xlsx
@@ -106,9 +106,6 @@
     <t>iaest-measure:municipio</t>
   </si>
   <si>
-    <t>iaest-measure:direccion-provincial-nombre</t>
-  </si>
-  <si>
     <t>sdmx-dimension:refPeriod</t>
   </si>
   <si>
@@ -128,6 +125,9 @@
   </si>
   <si>
     <t>xsd:string</t>
+  </si>
+  <si>
+    <t>URI-Provincia</t>
   </si>
   <si>
     <t>xsd:date</t>
@@ -137,20 +137,30 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -164,11 +174,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment/>
     </xf>
   </cellXfs>
@@ -297,20 +310,20 @@
       <c r="H3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4">
@@ -321,22 +334,22 @@
         <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="E4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>33</v>
@@ -351,7 +364,7 @@
         <v>26</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5">
@@ -362,22 +375,22 @@
         <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>38</v>

</xml_diff>